<commit_message>
modified track data to include red yard block
</commit_message>
<xml_diff>
--- a/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
+++ b/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="93">
   <si>
     <t>Sections consist of multiple blocks.</t>
   </si>
@@ -1540,7 +1540,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:L155"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -1596,21 +1596,21 @@
       <c r="K1" s="33"/>
       <c r="L1" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="20">
         <v>50</v>
       </c>
       <c r="E2" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="20">
         <v>40</v>
@@ -1618,12 +1618,12 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="21">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J2" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="K2" s="18"/>
+        <v>4.13</v>
+      </c>
+      <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
@@ -1633,14 +1633,14 @@
       <c r="B3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="20">
-        <v>2</v>
+      <c r="C3" s="19">
+        <v>1</v>
       </c>
       <c r="D3" s="20">
         <v>50</v>
       </c>
-      <c r="E3" s="20">
-        <v>1</v>
+      <c r="E3" s="21">
+        <v>0.5</v>
       </c>
       <c r="F3" s="20">
         <v>40</v>
@@ -1648,10 +1648,10 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="21">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="J3" s="21">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="7"/>
@@ -1664,13 +1664,13 @@
         <v>16</v>
       </c>
       <c r="C4" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="20">
         <v>50</v>
       </c>
-      <c r="E4" s="21">
-        <v>1.5</v>
+      <c r="E4" s="20">
+        <v>1</v>
       </c>
       <c r="F4" s="20">
         <v>40</v>
@@ -1678,29 +1678,29 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="21">
         <v>0.75</v>
       </c>
-      <c r="J4" s="21">
-        <v>1.5</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="25"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="19">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="20">
+        <v>3</v>
       </c>
       <c r="D5" s="20">
         <v>50</v>
       </c>
-      <c r="E5" s="20">
-        <v>2</v>
+      <c r="E5" s="21">
+        <v>1.5</v>
       </c>
       <c r="F5" s="20">
         <v>40</v>
@@ -1708,13 +1708,13 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="21">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J5" s="21">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="18" t="s">
@@ -1723,14 +1723,14 @@
       <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="20">
-        <v>5</v>
+      <c r="C6" s="19">
+        <v>4</v>
       </c>
       <c r="D6" s="20">
         <v>50</v>
       </c>
-      <c r="E6" s="21">
-        <v>1.5</v>
+      <c r="E6" s="20">
+        <v>2</v>
       </c>
       <c r="F6" s="20">
         <v>40</v>
@@ -1738,10 +1738,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="21">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J6" s="21">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -1754,13 +1754,13 @@
         <v>19</v>
       </c>
       <c r="C7" s="20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="20">
         <v>50</v>
       </c>
-      <c r="E7" s="20">
-        <v>1</v>
+      <c r="E7" s="21">
+        <v>1.5</v>
       </c>
       <c r="F7" s="20">
         <v>40</v>
@@ -1768,10 +1768,10 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="21">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J7" s="21">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -1781,31 +1781,27 @@
         <v>66</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="19">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="20">
+        <v>6</v>
       </c>
       <c r="D8" s="20">
-        <v>75</v>
-      </c>
-      <c r="E8" s="21">
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1</v>
       </c>
       <c r="F8" s="20">
         <v>40</v>
       </c>
-      <c r="G8" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="21">
-        <v>0.38</v>
+        <v>0.5</v>
       </c>
       <c r="J8" s="21">
-        <v>4.13</v>
+        <v>3.75</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -1817,22 +1813,26 @@
       <c r="B9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="20">
-        <v>8</v>
+      <c r="C9" s="19">
+        <v>7</v>
       </c>
       <c r="D9" s="20">
         <v>75</v>
       </c>
-      <c r="E9" s="20">
-        <v>0</v>
+      <c r="E9" s="21">
+        <v>0.5</v>
       </c>
       <c r="F9" s="20">
         <v>40</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I9" s="21">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="J9" s="21">
         <v>4.13</v>
@@ -1848,7 +1848,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="20">
         <v>75</v>
@@ -1859,9 +1859,7 @@
       <c r="F10" s="20">
         <v>40</v>
       </c>
-      <c r="G10" s="24" t="s">
-        <v>68</v>
-      </c>
+      <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="21">
         <v>0</v>
@@ -1877,10 +1875,10 @@
         <v>66</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="19">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="20">
+        <v>9</v>
       </c>
       <c r="D11" s="20">
         <v>75</v>
@@ -1891,7 +1889,9 @@
       <c r="F11" s="20">
         <v>40</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="21">
         <v>0</v>
@@ -1909,14 +1909,14 @@
       <c r="B12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="20">
-        <v>11</v>
+      <c r="C12" s="19">
+        <v>10</v>
       </c>
       <c r="D12" s="20">
         <v>75</v>
       </c>
-      <c r="E12" s="21">
-        <v>-0.5</v>
+      <c r="E12" s="20">
+        <v>0</v>
       </c>
       <c r="F12" s="20">
         <v>40</v>
@@ -1924,10 +1924,10 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="21">
-        <v>-0.38</v>
+        <v>0</v>
       </c>
       <c r="J12" s="21">
-        <v>3.75</v>
+        <v>4.13</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1939,14 +1939,14 @@
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="19">
-        <v>12</v>
+      <c r="C13" s="20">
+        <v>11</v>
       </c>
       <c r="D13" s="20">
         <v>75</v>
       </c>
-      <c r="E13" s="20">
-        <v>-1</v>
+      <c r="E13" s="21">
+        <v>-0.5</v>
       </c>
       <c r="F13" s="20">
         <v>40</v>
@@ -1954,10 +1954,10 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="21">
-        <v>-0.75</v>
+        <v>-0.38</v>
       </c>
       <c r="J13" s="21">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -1967,16 +1967,16 @@
         <v>66</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="20">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="C14" s="19">
+        <v>12</v>
       </c>
       <c r="D14" s="20">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E14" s="20">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F14" s="20">
         <v>40</v>
@@ -1984,10 +1984,10 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="21">
-        <v>-1.4</v>
+        <v>-0.75</v>
       </c>
       <c r="J14" s="21">
-        <v>1.6</v>
+        <v>3</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -2000,13 +2000,13 @@
         <v>26</v>
       </c>
       <c r="C15" s="20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="20">
-        <v>60</v>
-      </c>
-      <c r="E15" s="21">
-        <v>-1.25</v>
+        <v>70</v>
+      </c>
+      <c r="E15" s="20">
+        <v>-2</v>
       </c>
       <c r="F15" s="20">
         <v>40</v>
@@ -2014,10 +2014,10 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="21">
-        <v>-0.75</v>
+        <v>-1.4</v>
       </c>
       <c r="J15" s="21">
-        <v>0.85</v>
+        <v>1.6</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -2029,27 +2029,25 @@
       <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19">
-        <v>15</v>
+      <c r="C16" s="20">
+        <v>14</v>
       </c>
       <c r="D16" s="20">
         <v>60</v>
       </c>
-      <c r="E16" s="20">
-        <v>-1</v>
+      <c r="E16" s="21">
+        <v>-1.25</v>
       </c>
       <c r="F16" s="20">
         <v>40</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>69</v>
-      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="21">
-        <v>-0.6</v>
+        <v>-0.75</v>
       </c>
       <c r="J16" s="21">
-        <v>0.25</v>
+        <v>0.85</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -2059,31 +2057,29 @@
         <v>66</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="20">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="C17" s="19">
+        <v>15</v>
       </c>
       <c r="D17" s="20">
-        <v>50</v>
-      </c>
-      <c r="E17" s="21">
-        <v>-0.5</v>
+        <v>60</v>
+      </c>
+      <c r="E17" s="20">
+        <v>-1</v>
       </c>
       <c r="F17" s="20">
         <v>40</v>
       </c>
-      <c r="G17" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="7"/>
       <c r="I17" s="21">
-        <v>-0.25</v>
+        <v>-0.6</v>
       </c>
       <c r="J17" s="21">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -2095,25 +2091,29 @@
       <c r="B18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="19">
-        <v>17</v>
+      <c r="C18" s="20">
+        <v>16</v>
       </c>
       <c r="D18" s="20">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E18" s="21">
         <v>-0.5</v>
       </c>
       <c r="F18" s="20">
-        <v>55</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I18" s="21">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="J18" s="21">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -2125,25 +2125,25 @@
       <c r="B19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="20">
-        <v>18</v>
+      <c r="C19" s="19">
+        <v>17</v>
       </c>
       <c r="D19" s="20">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E19" s="21">
-        <v>-0.06</v>
+        <v>-0.5</v>
       </c>
       <c r="F19" s="20">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="21">
-        <v>-0.24</v>
+        <v>-1</v>
       </c>
       <c r="J19" s="21">
-        <v>-1.24</v>
+        <v>-1</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -2156,13 +2156,13 @@
         <v>28</v>
       </c>
       <c r="C20" s="20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="20">
         <v>400</v>
       </c>
-      <c r="E20" s="20">
-        <v>0</v>
+      <c r="E20" s="21">
+        <v>-0.06</v>
       </c>
       <c r="F20" s="20">
         <v>70</v>
@@ -2170,7 +2170,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="21">
-        <v>0</v>
+        <v>-0.24</v>
       </c>
       <c r="J20" s="21">
         <v>-1.24</v>
@@ -2185,11 +2185,11 @@
       <c r="B21" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="19">
-        <v>20</v>
+      <c r="C21" s="20">
+        <v>19</v>
       </c>
       <c r="D21" s="20">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E21" s="20">
         <v>0</v>
@@ -2213,26 +2213,22 @@
         <v>66</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="20">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="C22" s="19">
+        <v>20</v>
       </c>
       <c r="D22" s="20">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E22" s="20">
         <v>0</v>
       </c>
       <c r="F22" s="20">
-        <v>55</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>25</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="21">
         <v>0</v>
       </c>
@@ -2249,8 +2245,8 @@
       <c r="B23" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="19">
-        <v>22</v>
+      <c r="C23" s="20">
+        <v>21</v>
       </c>
       <c r="D23" s="20">
         <v>100</v>
@@ -2261,8 +2257,12 @@
       <c r="F23" s="20">
         <v>55</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="G23" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I23" s="21">
         <v>0</v>
       </c>
@@ -2279,8 +2279,8 @@
       <c r="B24" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="20">
-        <v>23</v>
+      <c r="C24" s="19">
+        <v>22</v>
       </c>
       <c r="D24" s="20">
         <v>100</v>
@@ -2307,23 +2307,21 @@
         <v>66</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="20">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="20">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E25" s="20">
         <v>0</v>
       </c>
       <c r="F25" s="20">
-        <v>70</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>35</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="21">
         <v>0</v>
@@ -2341,8 +2339,8 @@
       <c r="B26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="19">
-        <v>25</v>
+      <c r="C26" s="20">
+        <v>24</v>
       </c>
       <c r="D26" s="20">
         <v>50</v>
@@ -2353,12 +2351,10 @@
       <c r="F26" s="20">
         <v>70</v>
       </c>
-      <c r="G26" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="7"/>
       <c r="I26" s="21">
         <v>0</v>
       </c>
@@ -2368,15 +2364,15 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="20">
-        <v>26</v>
+      <c r="C27" s="19">
+        <v>25</v>
       </c>
       <c r="D27" s="20">
         <v>50</v>
@@ -2387,10 +2383,12 @@
       <c r="F27" s="20">
         <v>70</v>
       </c>
-      <c r="G27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="7"/>
+      <c r="G27" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I27" s="21">
         <v>0</v>
       </c>
@@ -2407,8 +2405,8 @@
       <c r="B28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="19">
-        <v>27</v>
+      <c r="C28" s="20">
+        <v>26</v>
       </c>
       <c r="D28" s="20">
         <v>50</v>
@@ -2419,8 +2417,8 @@
       <c r="F28" s="20">
         <v>70</v>
       </c>
-      <c r="G28" s="24" t="s">
-        <v>73</v>
+      <c r="G28" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="21">
@@ -2439,8 +2437,8 @@
       <c r="B29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="20">
-        <v>28</v>
+      <c r="C29" s="19">
+        <v>27</v>
       </c>
       <c r="D29" s="20">
         <v>50</v>
@@ -2451,8 +2449,8 @@
       <c r="F29" s="20">
         <v>70</v>
       </c>
-      <c r="G29" s="18" t="s">
-        <v>35</v>
+      <c r="G29" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="21">
@@ -2472,10 +2470,10 @@
         <v>33</v>
       </c>
       <c r="C30" s="20">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="20">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E30" s="20">
         <v>0</v>
@@ -2503,8 +2501,8 @@
       <c r="B31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="19">
-        <v>30</v>
+      <c r="C31" s="20">
+        <v>29</v>
       </c>
       <c r="D31" s="20">
         <v>60</v>
@@ -2535,11 +2533,11 @@
       <c r="B32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="20">
-        <v>31</v>
+      <c r="C32" s="19">
+        <v>30</v>
       </c>
       <c r="D32" s="20">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E32" s="20">
         <v>0</v>
@@ -2567,8 +2565,8 @@
       <c r="B33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="19">
-        <v>32</v>
+      <c r="C33" s="20">
+        <v>31</v>
       </c>
       <c r="D33" s="20">
         <v>50</v>
@@ -2599,8 +2597,8 @@
       <c r="B34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="20">
-        <v>33</v>
+      <c r="C34" s="19">
+        <v>32</v>
       </c>
       <c r="D34" s="20">
         <v>50</v>
@@ -2612,7 +2610,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="21">
@@ -2632,7 +2630,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="20">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="20">
         <v>50</v>
@@ -2644,7 +2642,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="21">
@@ -2663,8 +2661,8 @@
       <c r="B36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="19">
-        <v>35</v>
+      <c r="C36" s="20">
+        <v>34</v>
       </c>
       <c r="D36" s="20">
         <v>50</v>
@@ -2675,12 +2673,10 @@
       <c r="F36" s="20">
         <v>70</v>
       </c>
-      <c r="G36" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G36" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="7"/>
       <c r="I36" s="21">
         <v>0</v>
       </c>
@@ -2697,8 +2693,8 @@
       <c r="B37" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="20">
-        <v>36</v>
+      <c r="C37" s="19">
+        <v>35</v>
       </c>
       <c r="D37" s="20">
         <v>50</v>
@@ -2709,10 +2705,12 @@
       <c r="F37" s="20">
         <v>70</v>
       </c>
-      <c r="G37" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" s="7"/>
+      <c r="G37" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I37" s="21">
         <v>0</v>
       </c>
@@ -2730,7 +2728,7 @@
         <v>33</v>
       </c>
       <c r="C38" s="20">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="20">
         <v>50</v>
@@ -2761,8 +2759,8 @@
       <c r="B39" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="19">
-        <v>38</v>
+      <c r="C39" s="20">
+        <v>37</v>
       </c>
       <c r="D39" s="20">
         <v>50</v>
@@ -2773,8 +2771,8 @@
       <c r="F39" s="20">
         <v>70</v>
       </c>
-      <c r="G39" s="24" t="s">
-        <v>76</v>
+      <c r="G39" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="21">
@@ -2793,8 +2791,8 @@
       <c r="B40" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="20">
-        <v>39</v>
+      <c r="C40" s="19">
+        <v>38</v>
       </c>
       <c r="D40" s="20">
         <v>50</v>
@@ -2805,8 +2803,8 @@
       <c r="F40" s="20">
         <v>70</v>
       </c>
-      <c r="G40" s="18" t="s">
-        <v>35</v>
+      <c r="G40" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="21">
@@ -2826,10 +2824,10 @@
         <v>33</v>
       </c>
       <c r="C41" s="20">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="20">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E41" s="20">
         <v>0</v>
@@ -2857,8 +2855,8 @@
       <c r="B42" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19">
-        <v>41</v>
+      <c r="C42" s="20">
+        <v>40</v>
       </c>
       <c r="D42" s="20">
         <v>60</v>
@@ -2889,11 +2887,11 @@
       <c r="B43" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="20">
-        <v>42</v>
+      <c r="C43" s="19">
+        <v>41</v>
       </c>
       <c r="D43" s="20">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E43" s="20">
         <v>0</v>
@@ -2922,7 +2920,7 @@
         <v>33</v>
       </c>
       <c r="C44" s="20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="20">
         <v>50</v>
@@ -2933,7 +2931,7 @@
       <c r="F44" s="20">
         <v>70</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G44" s="18" t="s">
         <v>35</v>
       </c>
       <c r="H44" s="7"/>
@@ -2953,8 +2951,8 @@
       <c r="B45" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="19">
-        <v>44</v>
+      <c r="C45" s="20">
+        <v>43</v>
       </c>
       <c r="D45" s="20">
         <v>50</v>
@@ -2965,8 +2963,8 @@
       <c r="F45" s="20">
         <v>70</v>
       </c>
-      <c r="G45" s="18" t="s">
-        <v>77</v>
+      <c r="G45" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="21">
@@ -2985,8 +2983,8 @@
       <c r="B46" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="20">
-        <v>45</v>
+      <c r="C46" s="19">
+        <v>44</v>
       </c>
       <c r="D46" s="20">
         <v>50</v>
@@ -2997,12 +2995,10 @@
       <c r="F46" s="20">
         <v>70</v>
       </c>
-      <c r="G46" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G46" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="7"/>
       <c r="I46" s="21">
         <v>0</v>
       </c>
@@ -3017,13 +3013,13 @@
         <v>66</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C47" s="20">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="20">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E47" s="20">
         <v>0</v>
@@ -3031,10 +3027,12 @@
       <c r="F47" s="20">
         <v>70</v>
       </c>
-      <c r="G47" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H47" s="7"/>
+      <c r="G47" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I47" s="21">
         <v>0</v>
       </c>
@@ -3051,8 +3049,8 @@
       <c r="B48" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="19">
-        <v>47</v>
+      <c r="C48" s="20">
+        <v>46</v>
       </c>
       <c r="D48" s="20">
         <v>75</v>
@@ -3063,8 +3061,8 @@
       <c r="F48" s="20">
         <v>70</v>
       </c>
-      <c r="G48" s="24" t="s">
-        <v>27</v>
+      <c r="G48" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="21">
@@ -3083,8 +3081,8 @@
       <c r="B49" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="20">
-        <v>48</v>
+      <c r="C49" s="19">
+        <v>47</v>
       </c>
       <c r="D49" s="20">
         <v>75</v>
@@ -3096,11 +3094,9 @@
         <v>70</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H49" s="7"/>
       <c r="I49" s="21">
         <v>0</v>
       </c>
@@ -3115,22 +3111,26 @@
         <v>66</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C50" s="20">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="20">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="E50" s="20">
         <v>0</v>
       </c>
       <c r="F50" s="20">
-        <v>60</v>
-      </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I50" s="21">
         <v>0</v>
       </c>
@@ -3147,8 +3147,8 @@
       <c r="B51" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="19">
-        <v>50</v>
+      <c r="C51" s="20">
+        <v>49</v>
       </c>
       <c r="D51" s="20">
         <v>50</v>
@@ -3177,8 +3177,8 @@
       <c r="B52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="20">
-        <v>51</v>
+      <c r="C52" s="19">
+        <v>50</v>
       </c>
       <c r="D52" s="20">
         <v>50</v>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="20">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -3208,10 +3208,10 @@
         <v>40</v>
       </c>
       <c r="C53" s="20">
-        <v>52</v>
-      </c>
-      <c r="D53" s="21">
-        <v>43.2</v>
+        <v>51</v>
+      </c>
+      <c r="D53" s="20">
+        <v>50</v>
       </c>
       <c r="E53" s="20">
         <v>0</v>
@@ -3219,9 +3219,7 @@
       <c r="F53" s="20">
         <v>55</v>
       </c>
-      <c r="G53" s="18" t="s">
-        <v>80</v>
-      </c>
+      <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="21">
         <v>0</v>
@@ -3239,11 +3237,11 @@
       <c r="B54" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="19">
-        <v>53</v>
-      </c>
-      <c r="D54" s="20">
-        <v>50</v>
+      <c r="C54" s="20">
+        <v>52</v>
+      </c>
+      <c r="D54" s="21">
+        <v>43.2</v>
       </c>
       <c r="E54" s="20">
         <v>0</v>
@@ -3251,7 +3249,9 @@
       <c r="F54" s="20">
         <v>55</v>
       </c>
-      <c r="G54" s="7"/>
+      <c r="G54" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="H54" s="7"/>
       <c r="I54" s="21">
         <v>0</v>
@@ -3269,8 +3269,8 @@
       <c r="B55" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C55" s="20">
-        <v>54</v>
+      <c r="C55" s="19">
+        <v>53</v>
       </c>
       <c r="D55" s="20">
         <v>50</v>
@@ -3297,16 +3297,16 @@
         <v>66</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C56" s="20">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="20">
-        <v>75</v>
-      </c>
-      <c r="E56" s="21">
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+      <c r="E56" s="20">
+        <v>0</v>
       </c>
       <c r="F56" s="20">
         <v>55</v>
@@ -3314,10 +3314,10 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="21">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="J56" s="21">
-        <v>-0.87</v>
+        <v>-1.24</v>
       </c>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
@@ -3329,8 +3329,8 @@
       <c r="B57" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="19">
-        <v>56</v>
+      <c r="C57" s="20">
+        <v>55</v>
       </c>
       <c r="D57" s="20">
         <v>75</v>
@@ -3347,7 +3347,7 @@
         <v>0.38</v>
       </c>
       <c r="J57" s="21">
-        <v>-0.49</v>
+        <v>-0.87</v>
       </c>
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
@@ -3359,8 +3359,8 @@
       <c r="B58" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="20">
-        <v>57</v>
+      <c r="C58" s="19">
+        <v>56</v>
       </c>
       <c r="D58" s="20">
         <v>75</v>
@@ -3377,7 +3377,7 @@
         <v>0.38</v>
       </c>
       <c r="J58" s="21">
-        <v>-0.12</v>
+        <v>-0.49</v>
       </c>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
@@ -3387,16 +3387,16 @@
         <v>66</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C59" s="20">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="20">
         <v>75</v>
       </c>
-      <c r="E59" s="20">
-        <v>1</v>
+      <c r="E59" s="21">
+        <v>0.5</v>
       </c>
       <c r="F59" s="20">
         <v>55</v>
@@ -3404,10 +3404,10 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="21">
-        <v>0.75</v>
+        <v>0.38</v>
       </c>
       <c r="J59" s="21">
-        <v>0.63</v>
+        <v>-0.12</v>
       </c>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
@@ -3419,14 +3419,14 @@
       <c r="B60" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="19">
-        <v>59</v>
+      <c r="C60" s="20">
+        <v>58</v>
       </c>
       <c r="D60" s="20">
         <v>75</v>
       </c>
-      <c r="E60" s="21">
-        <v>0.5</v>
+      <c r="E60" s="20">
+        <v>1</v>
       </c>
       <c r="F60" s="20">
         <v>55</v>
@@ -3434,10 +3434,10 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="21">
-        <v>0.38</v>
+        <v>0.75</v>
       </c>
       <c r="J60" s="21">
-        <v>1.01</v>
+        <v>0.63</v>
       </c>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
@@ -3449,26 +3449,22 @@
       <c r="B61" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C61" s="20">
-        <v>60</v>
+      <c r="C61" s="19">
+        <v>59</v>
       </c>
       <c r="D61" s="20">
         <v>75</v>
       </c>
-      <c r="E61" s="20">
-        <v>0</v>
+      <c r="E61" s="21">
+        <v>0.5</v>
       </c>
       <c r="F61" s="20">
         <v>55</v>
       </c>
-      <c r="G61" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H61" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
       <c r="I61" s="21">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="J61" s="21">
         <v>1.01</v>
@@ -3481,27 +3477,31 @@
         <v>66</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C62" s="20">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62" s="20">
         <v>75</v>
       </c>
-      <c r="E62" s="21">
-        <v>-0.5</v>
+      <c r="E62" s="20">
+        <v>0</v>
       </c>
       <c r="F62" s="20">
         <v>55</v>
       </c>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
+      <c r="G62" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I62" s="21">
-        <v>-0.38</v>
+        <v>0</v>
       </c>
       <c r="J62" s="21">
-        <v>0.63</v>
+        <v>1.01</v>
       </c>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -3513,14 +3513,14 @@
       <c r="B63" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="19">
-        <v>62</v>
+      <c r="C63" s="20">
+        <v>61</v>
       </c>
       <c r="D63" s="20">
         <v>75</v>
       </c>
-      <c r="E63" s="20">
-        <v>-1</v>
+      <c r="E63" s="21">
+        <v>-0.5</v>
       </c>
       <c r="F63" s="20">
         <v>55</v>
@@ -3528,10 +3528,10 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="21">
-        <v>-0.75</v>
+        <v>-0.38</v>
       </c>
       <c r="J63" s="21">
-        <v>-0.12</v>
+        <v>0.63</v>
       </c>
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
@@ -3543,8 +3543,8 @@
       <c r="B64" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="20">
-        <v>63</v>
+      <c r="C64" s="19">
+        <v>62</v>
       </c>
       <c r="D64" s="20">
         <v>75</v>
@@ -3561,7 +3561,7 @@
         <v>-0.75</v>
       </c>
       <c r="J64" s="21">
-        <v>-0.87</v>
+        <v>-0.12</v>
       </c>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
@@ -3571,16 +3571,16 @@
         <v>66</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C65" s="20">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65" s="20">
         <v>75</v>
       </c>
-      <c r="E65" s="21">
-        <v>-0.5</v>
+      <c r="E65" s="20">
+        <v>-1</v>
       </c>
       <c r="F65" s="20">
         <v>55</v>
@@ -3588,10 +3588,10 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="21">
-        <v>-0.38</v>
+        <v>-0.75</v>
       </c>
       <c r="J65" s="21">
-        <v>-1.24</v>
+        <v>-0.87</v>
       </c>
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
@@ -3603,14 +3603,14 @@
       <c r="B66" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C66" s="19">
-        <v>65</v>
+      <c r="C66" s="20">
+        <v>64</v>
       </c>
       <c r="D66" s="20">
         <v>75</v>
       </c>
-      <c r="E66" s="20">
-        <v>0</v>
+      <c r="E66" s="21">
+        <v>-0.5</v>
       </c>
       <c r="F66" s="20">
         <v>55</v>
@@ -3618,7 +3618,7 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="21">
-        <v>0</v>
+        <v>-0.38</v>
       </c>
       <c r="J66" s="21">
         <v>-1.24</v>
@@ -3633,8 +3633,8 @@
       <c r="B67" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C67" s="20">
-        <v>66</v>
+      <c r="C67" s="19">
+        <v>65</v>
       </c>
       <c r="D67" s="20">
         <v>75</v>
@@ -3661,13 +3661,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C68" s="20">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="20">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="E68" s="20">
         <v>0</v>
@@ -3675,9 +3675,7 @@
       <c r="F68" s="20">
         <v>55</v>
       </c>
-      <c r="G68" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="21">
         <v>0</v>
@@ -3693,10 +3691,10 @@
         <v>66</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="19">
-        <v>68</v>
+        <v>52</v>
+      </c>
+      <c r="C69" s="20">
+        <v>67</v>
       </c>
       <c r="D69" s="20">
         <v>50</v>
@@ -3727,8 +3725,8 @@
       <c r="B70" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C70" s="20">
-        <v>69</v>
+      <c r="C70" s="19">
+        <v>68</v>
       </c>
       <c r="D70" s="20">
         <v>50</v>
@@ -3760,7 +3758,7 @@
         <v>54</v>
       </c>
       <c r="C71" s="20">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D71" s="20">
         <v>50</v>
@@ -3789,10 +3787,10 @@
         <v>66</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C72" s="19">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="C72" s="20">
+        <v>70</v>
       </c>
       <c r="D72" s="20">
         <v>50</v>
@@ -3821,10 +3819,10 @@
         <v>66</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C73" s="20">
-        <v>72</v>
+        <v>56</v>
+      </c>
+      <c r="C73" s="19">
+        <v>71</v>
       </c>
       <c r="D73" s="20">
         <v>50</v>
@@ -3853,10 +3851,10 @@
         <v>66</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C74" s="20">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="20">
         <v>50</v>
@@ -3887,8 +3885,8 @@
       <c r="B75" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C75" s="19">
-        <v>74</v>
+      <c r="C75" s="20">
+        <v>73</v>
       </c>
       <c r="D75" s="20">
         <v>50</v>
@@ -3919,8 +3917,8 @@
       <c r="B76" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C76" s="20">
-        <v>75</v>
+      <c r="C76" s="19">
+        <v>74</v>
       </c>
       <c r="D76" s="20">
         <v>50</v>
@@ -3949,10 +3947,10 @@
         <v>66</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C77" s="20">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D77" s="20">
         <v>50</v>
@@ -3978,23 +3976,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" s="20">
+        <v>76</v>
+      </c>
+      <c r="D78" s="20">
+        <v>50</v>
+      </c>
+      <c r="E78" s="20">
+        <v>0</v>
+      </c>
+      <c r="F78" s="20">
+        <v>55</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="H78" s="7"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="28"/>
+      <c r="I78" s="21">
+        <v>0</v>
+      </c>
+      <c r="J78" s="21">
+        <v>-1.24</v>
+      </c>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="23">
-        <f>A78</f>
+      <c r="A79" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="19"/>
@@ -5207,6 +5221,22 @@
       <c r="J154" s="28"/>
       <c r="K154" s="7"/>
       <c r="L154" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+      <c r="A155" s="23">
+        <f>A154</f>
+      </c>
+      <c r="B155" s="7"/>
+      <c r="C155" s="19"/>
+      <c r="D155" s="27"/>
+      <c r="E155" s="27"/>
+      <c r="F155" s="27"/>
+      <c r="G155" s="7"/>
+      <c r="H155" s="7"/>
+      <c r="I155" s="28"/>
+      <c r="J155" s="28"/>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5290,7 +5320,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="20">
         <v>45</v>
@@ -5298,7 +5328,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J2" s="21">
         <v>0.5</v>
@@ -10284,7 +10314,7 @@
         <v>100</v>
       </c>
       <c r="E153" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F153" s="20">
         <v>45</v>
@@ -10292,7 +10322,7 @@
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
       <c r="I153" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J153" s="21">
         <v>0.5</v>

</xml_diff>

<commit_message>
red line occupancy logic added
</commit_message>
<xml_diff>
--- a/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
+++ b/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
@@ -229,10 +229,10 @@
     <t>SWITCH TO/FROM YARD (75-yard)</t>
   </si>
   <si>
-    <t>SWITCH (15-16; 1-16)</t>
+    <t/>
   </si>
   <si>
-    <t>STATION: HERRON AVE</t>
+    <t>STATION: HERRON AVE; SWITCH (15-16; 1-16)</t>
   </si>
   <si>
     <t>STATION: SWISSVILLE</t>
@@ -411,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -514,6 +514,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,7 +856,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="44" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="45" width="31.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="10" width="13.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -863,18 +866,18 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="42"/>
+      <c r="A2" s="43"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -894,8 +897,8 @@
       <c r="G3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -945,7 +948,7 @@
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -963,7 +966,7 @@
       <c r="G1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
@@ -991,7 +994,7 @@
         <v>50</v>
       </c>
       <c r="G2" s="19"/>
-      <c r="H2" s="37"/>
+      <c r="H2" s="38"/>
       <c r="I2" s="22">
         <f>E2*D2/100</f>
       </c>
@@ -1019,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="19"/>
-      <c r="H3" s="37"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="22">
         <f>E3*D3/100</f>
       </c>
@@ -1047,7 +1050,7 @@
         <v>50</v>
       </c>
       <c r="G4" s="19"/>
-      <c r="H4" s="37"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="22">
         <f>E4*D4/100</f>
       </c>
@@ -1075,7 +1078,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="19"/>
-      <c r="H5" s="37"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="22">
         <f>E5*D5/100</f>
       </c>
@@ -1105,7 +1108,7 @@
       <c r="G6" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="22">
         <f>E6*D6/100</f>
       </c>
@@ -1135,7 +1138,7 @@
       <c r="G7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="22">
         <f>E7*D7/100</f>
       </c>
@@ -1163,7 +1166,7 @@
         <v>50</v>
       </c>
       <c r="G8" s="19"/>
-      <c r="H8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="22">
         <f>E8*D8/100</f>
       </c>
@@ -1191,7 +1194,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="19"/>
-      <c r="H9" s="37"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="22">
         <f>E9*D9/100</f>
       </c>
@@ -1219,7 +1222,7 @@
         <v>50</v>
       </c>
       <c r="G10" s="19"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="22">
         <f>E10*D10/100</f>
       </c>
@@ -1249,7 +1252,7 @@
       <c r="G11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="37"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="22">
         <f>E11*D11/100</f>
       </c>
@@ -1279,7 +1282,7 @@
       <c r="G12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="22">
         <f>E12*D12/100</f>
       </c>
@@ -1307,7 +1310,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="19"/>
-      <c r="H13" s="37"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="22">
         <f>E13*D13/100</f>
       </c>
@@ -1335,7 +1338,7 @@
         <v>50</v>
       </c>
       <c r="G14" s="19"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="22">
         <f>E14*D14/100</f>
       </c>
@@ -1363,7 +1366,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="22">
         <f>E15*D15/100</f>
       </c>
@@ -1393,7 +1396,7 @@
       <c r="G16" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="37"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="22">
         <f>E16*D16/100</f>
       </c>
@@ -1458,7 +1461,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -1499,19 +1502,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3"/>
-      <c r="B25" s="39">
+      <c r="B25" s="40">
         <v>1</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="40">
         <v>2</v>
       </c>
-      <c r="D25" s="39">
+      <c r="D25" s="40">
         <v>3</v>
       </c>
-      <c r="E25" s="39">
+      <c r="E25" s="40">
         <v>4</v>
       </c>
-      <c r="F25" s="39">
+      <c r="F25" s="40">
         <v>5</v>
       </c>
       <c r="G25" s="7"/>
@@ -1553,7 +1556,7 @@
   <cols>
     <col min="1" max="1" style="11" width="8.719285714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="10" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="8.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="36" width="8.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="32" width="11.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="32" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="32" width="13.290714285714287" customWidth="1" bestFit="1"/>
@@ -2074,7 +2077,7 @@
       <c r="F17" s="21">
         <v>40</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="35" t="s">
         <v>69</v>
       </c>
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
Made some changes to the signals
</commit_message>
<xml_diff>
--- a/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
+++ b/src/main/TrackModel/Track Layout & Vehicle Data vF2.xlsx
@@ -229,10 +229,10 @@
     <t>SWITCH TO/FROM YARD (75-yard)</t>
   </si>
   <si>
-    <t>SWITCH (15-16; 1-16)</t>
+    <t/>
   </si>
   <si>
-    <t>STATION: HERRON AVE</t>
+    <t>STATION: HERRON AVE; SWITCH (15-16; 1-16)</t>
   </si>
   <si>
     <t>STATION: SWISSVILLE</t>
@@ -411,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -514,6 +514,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,7 +856,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="44" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="45" width="31.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="10" width="13.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -863,18 +866,18 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="42"/>
+      <c r="A2" s="43"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -894,8 +897,8 @@
       <c r="G3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -945,7 +948,7 @@
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -963,7 +966,7 @@
       <c r="G1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
@@ -991,7 +994,7 @@
         <v>50</v>
       </c>
       <c r="G2" s="19"/>
-      <c r="H2" s="37"/>
+      <c r="H2" s="38"/>
       <c r="I2" s="22">
         <f>E2*D2/100</f>
       </c>
@@ -1019,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="19"/>
-      <c r="H3" s="37"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="22">
         <f>E3*D3/100</f>
       </c>
@@ -1047,7 +1050,7 @@
         <v>50</v>
       </c>
       <c r="G4" s="19"/>
-      <c r="H4" s="37"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="22">
         <f>E4*D4/100</f>
       </c>
@@ -1075,7 +1078,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="19"/>
-      <c r="H5" s="37"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="22">
         <f>E5*D5/100</f>
       </c>
@@ -1105,7 +1108,7 @@
       <c r="G6" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="22">
         <f>E6*D6/100</f>
       </c>
@@ -1135,7 +1138,7 @@
       <c r="G7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="22">
         <f>E7*D7/100</f>
       </c>
@@ -1163,7 +1166,7 @@
         <v>50</v>
       </c>
       <c r="G8" s="19"/>
-      <c r="H8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="22">
         <f>E8*D8/100</f>
       </c>
@@ -1191,7 +1194,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="19"/>
-      <c r="H9" s="37"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="22">
         <f>E9*D9/100</f>
       </c>
@@ -1219,7 +1222,7 @@
         <v>50</v>
       </c>
       <c r="G10" s="19"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="22">
         <f>E10*D10/100</f>
       </c>
@@ -1249,7 +1252,7 @@
       <c r="G11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="37"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="22">
         <f>E11*D11/100</f>
       </c>
@@ -1279,7 +1282,7 @@
       <c r="G12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="37"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="22">
         <f>E12*D12/100</f>
       </c>
@@ -1307,7 +1310,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="19"/>
-      <c r="H13" s="37"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="22">
         <f>E13*D13/100</f>
       </c>
@@ -1335,7 +1338,7 @@
         <v>50</v>
       </c>
       <c r="G14" s="19"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="22">
         <f>E14*D14/100</f>
       </c>
@@ -1363,7 +1366,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="22">
         <f>E15*D15/100</f>
       </c>
@@ -1393,7 +1396,7 @@
       <c r="G16" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="37"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="22">
         <f>E16*D16/100</f>
       </c>
@@ -1458,7 +1461,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="29"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -1499,19 +1502,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3"/>
-      <c r="B25" s="39">
+      <c r="B25" s="40">
         <v>1</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="40">
         <v>2</v>
       </c>
-      <c r="D25" s="39">
+      <c r="D25" s="40">
         <v>3</v>
       </c>
-      <c r="E25" s="39">
+      <c r="E25" s="40">
         <v>4</v>
       </c>
-      <c r="F25" s="39">
+      <c r="F25" s="40">
         <v>5</v>
       </c>
       <c r="G25" s="7"/>
@@ -1553,7 +1556,7 @@
   <cols>
     <col min="1" max="1" style="11" width="8.719285714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="10" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="8.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="36" width="8.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="32" width="11.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="32" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="32" width="13.290714285714287" customWidth="1" bestFit="1"/>
@@ -2074,7 +2077,7 @@
       <c r="F17" s="21">
         <v>40</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="35" t="s">
         <v>69</v>
       </c>
       <c r="H17" s="7"/>

</xml_diff>